<commit_message>
Better organize the clustering method.
</commit_message>
<xml_diff>
--- a/data/output/cluster_metrics_dbscan.xlsx
+++ b/data/output/cluster_metrics_dbscan.xlsx
@@ -482,12 +482,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>qa_fix_dispersion_mean</t>
+          <t>coldread_stopwatch_wpm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2.17e-13</t>
+          <t>nan</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved the prompt and added method to select different clustering for the prompt.
</commit_message>
<xml_diff>
--- a/data/output/cluster_metrics_dbscan.xlsx
+++ b/data/output/cluster_metrics_dbscan.xlsx
@@ -472,22 +472,18 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.3698858439812254</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.3204520461302064</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>coldread_stopwatch_wpm</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>